<commit_message>
Search functions in the DAOs
</commit_message>
<xml_diff>
--- a/todo.xlsx
+++ b/todo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\itu\Documents\S4\web-dynamique\gotta-taste-work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\ITU\S4\web-dynamique\gotta-taste-work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDB0513-9B50-4C9E-8F91-0F10B508CA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4EDAA7B-F506-4FE3-9FA8-652C33401F02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F12DE2D-7F2E-4E9C-B700-53BD58DE0CC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4F12DE2D-7F2E-4E9C-B700-53BD58DE0CC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="44">
   <si>
     <t>Identification du projet</t>
   </si>
@@ -138,13 +138,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>en cours</t>
-  </si>
-  <si>
     <t>terminé</t>
-  </si>
-  <si>
-    <t>à faire</t>
   </si>
   <si>
     <t>Choix des 4 entités</t>
@@ -254,7 +248,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -273,27 +267,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -609,19 +582,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072C5090-9705-49AC-B11D-59669D66D18E}">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52:D57"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="41.6640625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="41.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="47.21875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="20.77734375" style="9" customWidth="1"/>
+    <col min="1" max="2" width="47.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="9" customWidth="1"/>
     <col min="4" max="4" width="22" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="41.6640625" style="4"/>
+    <col min="5" max="16384" width="41.7109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -635,7 +608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -644,10 +617,10 @@
         <v>1000.0208333333334</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
@@ -656,10 +629,10 @@
         <v>1000.0416666666666</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -668,10 +641,10 @@
         <v>1000.0416666666666</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -680,22 +653,22 @@
         <v>1000.0104166666666</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="8">
         <v>1000.0020833333333</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>7</v>
       </c>
@@ -706,10 +679,10 @@
         <v>1000.0104166666666</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="11"/>
       <c r="B8" s="3" t="s">
         <v>30</v>
@@ -718,10 +691,10 @@
         <v>1000.0104166666666</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="11"/>
       <c r="B9" s="3" t="s">
         <v>31</v>
@@ -730,10 +703,10 @@
         <v>1000.0138888888889</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="11"/>
       <c r="B10" s="3" t="s">
         <v>32</v>
@@ -742,10 +715,10 @@
         <v>1000.0104166666666</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="11"/>
       <c r="B11" s="3" t="s">
         <v>33</v>
@@ -754,10 +727,10 @@
         <v>1000.0104166666666</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
       <c r="B12" s="3" t="s">
         <v>34</v>
@@ -766,10 +739,10 @@
         <v>1000.0104166666666</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
@@ -780,10 +753,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="B14" s="3" t="s">
         <v>30</v>
@@ -792,10 +765,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="11"/>
       <c r="B15" s="3" t="s">
         <v>31</v>
@@ -804,10 +777,10 @@
         <v>1000.0069444444445</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="11"/>
       <c r="B16" s="3" t="s">
         <v>32</v>
@@ -816,10 +789,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="11"/>
       <c r="B17" s="3" t="s">
         <v>33</v>
@@ -828,10 +801,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="11"/>
       <c r="B18" s="3" t="s">
         <v>34</v>
@@ -840,10 +813,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>10</v>
       </c>
@@ -854,10 +827,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="11"/>
       <c r="B20" s="3" t="s">
         <v>30</v>
@@ -866,10 +839,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="11"/>
       <c r="B21" s="3" t="s">
         <v>31</v>
@@ -878,10 +851,10 @@
         <v>1000.0069444444445</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="11"/>
       <c r="B22" s="3" t="s">
         <v>32</v>
@@ -890,10 +863,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="3" t="s">
         <v>33</v>
@@ -902,10 +875,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="3" t="s">
         <v>34</v>
@@ -914,12 +887,12 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>29</v>
@@ -928,10 +901,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="11"/>
       <c r="B26" s="3" t="s">
         <v>30</v>
@@ -940,10 +913,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="11"/>
       <c r="B27" s="3" t="s">
         <v>31</v>
@@ -952,10 +925,10 @@
         <v>1000.0069444444445</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="11"/>
       <c r="B28" s="3" t="s">
         <v>32</v>
@@ -964,10 +937,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="11"/>
       <c r="B29" s="3" t="s">
         <v>33</v>
@@ -976,10 +949,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
       <c r="B30" s="3" t="s">
         <v>34</v>
@@ -988,10 +961,10 @@
         <v>1000.0034722222222</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>11</v>
       </c>
@@ -1002,10 +975,10 @@
         <v>1001.0104166666666</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>12</v>
       </c>
@@ -1016,10 +989,10 @@
         <v>1001.0138888888889</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="3" t="s">
         <v>14</v>
@@ -1028,10 +1001,10 @@
         <v>1001.0069444444445</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="11"/>
       <c r="B34" s="3" t="s">
         <v>15</v>
@@ -1040,22 +1013,22 @@
         <v>1001.0069444444445</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C35" s="8">
         <v>1001.0069444444445</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="3" t="s">
         <v>16</v>
@@ -1064,10 +1037,10 @@
         <v>1001.0138888888889</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="3" t="s">
         <v>18</v>
@@ -1076,10 +1049,10 @@
         <v>1001.0069444444445</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="11"/>
       <c r="B38" s="3" t="s">
         <v>17</v>
@@ -1088,22 +1061,22 @@
         <v>1001.0069444444445</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="11"/>
       <c r="B39" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C39" s="8">
         <v>1001.0069444444445</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="11"/>
       <c r="B40" s="3" t="s">
         <v>27</v>
@@ -1112,10 +1085,10 @@
         <v>1001.0104166666666</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>26</v>
       </c>
@@ -1126,10 +1099,10 @@
         <v>1001.0208333333334</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="11"/>
       <c r="B42" s="3" t="s">
         <v>20</v>
@@ -1138,10 +1111,10 @@
         <v>1001.0069444444445</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="11"/>
       <c r="B43" s="3" t="s">
         <v>21</v>
@@ -1150,22 +1123,22 @@
         <v>1001.0069444444445</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C44" s="8">
         <v>1001.0069444444445</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="3" t="s">
         <v>23</v>
@@ -1174,10 +1147,10 @@
         <v>1001.0208333333334</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="11"/>
       <c r="B46" s="3" t="s">
         <v>24</v>
@@ -1186,10 +1159,10 @@
         <v>1001.0069444444445</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="11"/>
       <c r="B47" s="3" t="s">
         <v>25</v>
@@ -1198,22 +1171,22 @@
         <v>1001.0069444444445</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="11"/>
       <c r="B48" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C48" s="8">
         <v>1001.0069444444445</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="11"/>
       <c r="B49" s="3" t="s">
         <v>28</v>
@@ -1222,10 +1195,10 @@
         <v>1001.0104166666666</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>22</v>
       </c>
@@ -1236,10 +1209,10 @@
         <v>1002.0069444444445</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="11"/>
       <c r="B51" s="3" t="s">
         <v>20</v>
@@ -1248,10 +1221,10 @@
         <v>1002.0069444444445</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="11"/>
       <c r="B52" s="3" t="s">
         <v>21</v>
@@ -1260,22 +1233,22 @@
         <v>1002.0069444444445</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="11"/>
       <c r="B53" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C53" s="8">
         <v>1002.0069444444445</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="11"/>
       <c r="B54" s="3" t="s">
         <v>23</v>
@@ -1284,10 +1257,10 @@
         <v>1002.0069444444445</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="11"/>
       <c r="B55" s="3" t="s">
         <v>24</v>
@@ -1296,10 +1269,10 @@
         <v>1002.0069444444445</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="11"/>
       <c r="B56" s="3" t="s">
         <v>25</v>
@@ -1308,22 +1281,22 @@
         <v>1002.0069444444445</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="11"/>
       <c r="B57" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C57" s="8">
         <v>1002.0069444444445</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="11"/>
       <c r="B58" s="3" t="s">
         <v>28</v>
@@ -1332,10 +1305,10 @@
         <v>1002.0069444444445</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
         <v>36</v>
       </c>
@@ -1344,28 +1317,28 @@
         <f>SUM(C2:C58)</f>
         <v>57037.502083333362</v>
       </c>
-      <c r="D59" s="1" t="s">
+      <c r="D59" s="3" t="s">
         <v>37</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A41:A49"/>
+    <mergeCell ref="A50:A58"/>
     <mergeCell ref="A7:A12"/>
     <mergeCell ref="A13:A18"/>
     <mergeCell ref="A19:A24"/>
     <mergeCell ref="A25:A30"/>
     <mergeCell ref="A32:A40"/>
-    <mergeCell ref="A41:A49"/>
-    <mergeCell ref="A50:A58"/>
   </mergeCells>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="à faire">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="à faire">
       <formula>NOT(ISERROR(SEARCH("à faire",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="en cours">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="en cours">
       <formula>NOT(ISERROR(SEARCH("en cours",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="terminé">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="terminé">
       <formula>NOT(ISERROR(SEARCH("terminé",D1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>